<commit_message>
Problema 2 probably working, need to check with teacher
</commit_message>
<xml_diff>
--- a/fogos2/fogos2.xlsx
+++ b/fogos2/fogos2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\IncendioFlorestal\fogos2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23DB8952-0689-4364-A2A3-B010D1C9BCAA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD3C4AC-1443-46B2-B1D9-E6B22539F4D8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15990" windowHeight="6900" xr2:uid="{63F9166B-6F17-4C5E-B7E0-12EB27E8F6D8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8985" windowHeight="6795" xr2:uid="{63F9166B-6F17-4C5E-B7E0-12EB27E8F6D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,16 +27,10 @@
     <definedName name="t">Sheet1!$C$28:$I$34</definedName>
     <definedName name="x">Sheet1!$C$20:$I$26</definedName>
   </definedNames>
-  <calcPr calcId="191029" calcMode="manual"/>
+  <calcPr calcId="0" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -462,7 +456,7 @@
   <dimension ref="A2:Q34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,7 +530,7 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1">
         <v>10</v>
@@ -1128,7 +1122,7 @@
         <v>8</v>
       </c>
       <c r="C20" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" s="5">
         <v>1</v>
@@ -1137,7 +1131,7 @@
         <v>1</v>
       </c>
       <c r="F20" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20" s="5">
         <v>0</v>
@@ -1295,22 +1289,22 @@
         <v>0</v>
       </c>
       <c r="D28" s="5">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E28" s="5">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="F28" s="5">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G28" s="5">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H28" s="5">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="I28" s="5">
-        <v>63</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.25">
@@ -1318,137 +1312,137 @@
         <v>18</v>
       </c>
       <c r="D29" s="5">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E29" s="5">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="F29" s="5">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G29" s="5">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="H29" s="5">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="I29" s="5">
-        <v>73</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C30" s="5">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D30" s="5">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E30" s="5">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F30" s="5">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G30" s="5">
+        <v>62</v>
+      </c>
+      <c r="H30" s="5">
+        <v>66</v>
+      </c>
+      <c r="I30" s="5">
         <v>68</v>
-      </c>
-      <c r="H30" s="5">
-        <v>74</v>
-      </c>
-      <c r="I30" s="5">
-        <v>83</v>
       </c>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C31" s="5">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D31" s="5">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="E31" s="5">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F31" s="5">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G31" s="5">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="H31" s="5">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="I31" s="5">
-        <v>93</v>
+        <v>78</v>
       </c>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C32" s="5">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="D32" s="5">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E32" s="5">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F32" s="5">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G32" s="5">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="H32" s="5">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="I32" s="5">
-        <v>101</v>
+        <v>89</v>
       </c>
     </row>
     <row r="33" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C33" s="5">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="D33" s="5">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E33" s="5">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="F33" s="5">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G33" s="5">
+        <v>92</v>
+      </c>
+      <c r="H33" s="5">
+        <v>94</v>
+      </c>
+      <c r="I33" s="5">
         <v>97</v>
-      </c>
-      <c r="H33" s="5">
-        <v>102</v>
-      </c>
-      <c r="I33" s="5">
-        <v>111</v>
       </c>
     </row>
     <row r="34" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C34" s="5">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="D34" s="5">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="E34" s="5">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F34" s="5">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G34" s="5">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="H34" s="5">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="I34" s="5">
-        <v>120</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adicionado o fogos 3 e corrigida a função objetivo da 2
</commit_message>
<xml_diff>
--- a/fogos2/fogos2.xlsx
+++ b/fogos2/fogos2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\IncendioFlorestal\fogos2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD3C4AC-1443-46B2-B1D9-E6B22539F4D8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB50953-33B9-4456-A303-0D8E120FC3E9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="8985" windowHeight="6795" xr2:uid="{63F9166B-6F17-4C5E-B7E0-12EB27E8F6D8}"/>
   </bookViews>
@@ -530,7 +530,7 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1">
         <v>10</v>
@@ -1122,16 +1122,16 @@
         <v>8</v>
       </c>
       <c r="C20" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G20" s="5">
         <v>0</v>
@@ -1145,13 +1145,13 @@
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C21" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21" s="5">
         <v>0</v>
@@ -1168,10 +1168,10 @@
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C22" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22" s="5">
         <v>0</v>
@@ -1191,7 +1191,7 @@
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C23" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23" s="5">
         <v>0</v>
@@ -1289,160 +1289,160 @@
         <v>0</v>
       </c>
       <c r="D28" s="5">
+        <v>4</v>
+      </c>
+      <c r="E28" s="5">
+        <v>8</v>
+      </c>
+      <c r="F28" s="5">
         <v>12</v>
       </c>
-      <c r="E28" s="5">
-        <v>24</v>
-      </c>
-      <c r="F28" s="5">
-        <v>36</v>
-      </c>
       <c r="G28" s="5">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="H28" s="5">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="I28" s="5">
-        <v>52</v>
+        <v>18</v>
       </c>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C29" s="5">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D29" s="5">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="E29" s="5">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="F29" s="5">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="G29" s="5">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="H29" s="5">
-        <v>56</v>
+        <v>24</v>
       </c>
       <c r="I29" s="5">
-        <v>59</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C30" s="5">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="D30" s="5">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="E30" s="5">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="F30" s="5">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="G30" s="5">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="H30" s="5">
-        <v>66</v>
+        <v>34</v>
       </c>
       <c r="I30" s="5">
-        <v>68</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C31" s="5">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="D31" s="5">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="E31" s="5">
-        <v>68</v>
+        <v>36</v>
       </c>
       <c r="F31" s="5">
-        <v>70</v>
+        <v>38</v>
       </c>
       <c r="G31" s="5">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="H31" s="5">
-        <v>76</v>
+        <v>42</v>
       </c>
       <c r="I31" s="5">
-        <v>78</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C32" s="5">
-        <v>73</v>
+        <v>39</v>
       </c>
       <c r="D32" s="5">
-        <v>73</v>
+        <v>41</v>
       </c>
       <c r="E32" s="5">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="F32" s="5">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="G32" s="5">
-        <v>83</v>
+        <v>51</v>
       </c>
       <c r="H32" s="5">
-        <v>86</v>
+        <v>52</v>
       </c>
       <c r="I32" s="5">
-        <v>89</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C33" s="5">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="D33" s="5">
-        <v>84</v>
+        <v>52</v>
       </c>
       <c r="E33" s="5">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="F33" s="5">
-        <v>90</v>
+        <v>58</v>
       </c>
       <c r="G33" s="5">
-        <v>92</v>
+        <v>60</v>
       </c>
       <c r="H33" s="5">
-        <v>94</v>
+        <v>62</v>
       </c>
       <c r="I33" s="5">
-        <v>97</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C34" s="5">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="D34" s="5">
-        <v>95</v>
+        <v>61</v>
       </c>
       <c r="E34" s="5">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="F34" s="5">
-        <v>100</v>
+        <v>68</v>
       </c>
       <c r="G34" s="5">
-        <v>102</v>
+        <v>70</v>
       </c>
       <c r="H34" s="5">
-        <v>104</v>
+        <v>72</v>
       </c>
       <c r="I34" s="5">
-        <v>106</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adicionada a questão 2 ao relatório
</commit_message>
<xml_diff>
--- a/fogos2/fogos2.xlsx
+++ b/fogos2/fogos2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\IncendioFlorestal\fogos2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB50953-33B9-4456-A303-0D8E120FC3E9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1DF5EE2-8B0B-4BBD-8F2B-4C4E369268E3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="8985" windowHeight="6795" xr2:uid="{63F9166B-6F17-4C5E-B7E0-12EB27E8F6D8}"/>
   </bookViews>
@@ -1122,163 +1122,163 @@
         <v>8</v>
       </c>
       <c r="C20" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I20" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C23" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F23" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I23" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C24" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F24" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I24" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C25" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I25" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C26" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F26" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G26" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I26" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.25">
@@ -1289,160 +1289,160 @@
         <v>0</v>
       </c>
       <c r="D28" s="5">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E28" s="5">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="F28" s="5">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="G28" s="5">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="H28" s="5">
-        <v>16</v>
+        <v>54</v>
       </c>
       <c r="I28" s="5">
-        <v>18</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C29" s="5">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D29" s="5">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="E29" s="5">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="F29" s="5">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="G29" s="5">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="H29" s="5">
-        <v>24</v>
+        <v>72</v>
       </c>
       <c r="I29" s="5">
-        <v>26</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C30" s="5">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="D30" s="5">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="E30" s="5">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="F30" s="5">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="G30" s="5">
-        <v>30</v>
+        <v>78</v>
       </c>
       <c r="H30" s="5">
-        <v>34</v>
+        <v>90</v>
       </c>
       <c r="I30" s="5">
-        <v>33</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C31" s="5">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="D31" s="5">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="E31" s="5">
-        <v>36</v>
+        <v>76</v>
       </c>
       <c r="F31" s="5">
-        <v>38</v>
+        <v>86</v>
       </c>
       <c r="G31" s="5">
-        <v>40</v>
+        <v>96</v>
       </c>
       <c r="H31" s="5">
-        <v>42</v>
+        <v>108</v>
       </c>
       <c r="I31" s="5">
-        <v>42</v>
+        <v>116</v>
       </c>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C32" s="5">
-        <v>39</v>
+        <v>73</v>
       </c>
       <c r="D32" s="5">
-        <v>41</v>
+        <v>81</v>
       </c>
       <c r="E32" s="5">
-        <v>45</v>
+        <v>93</v>
       </c>
       <c r="F32" s="5">
-        <v>47</v>
+        <v>103</v>
       </c>
       <c r="G32" s="5">
-        <v>51</v>
+        <v>115</v>
       </c>
       <c r="H32" s="5">
-        <v>52</v>
+        <v>124</v>
       </c>
       <c r="I32" s="5">
-        <v>53</v>
+        <v>133</v>
       </c>
     </row>
     <row r="33" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C33" s="5">
-        <v>48</v>
+        <v>90</v>
       </c>
       <c r="D33" s="5">
-        <v>52</v>
+        <v>100</v>
       </c>
       <c r="E33" s="5">
-        <v>54</v>
+        <v>110</v>
       </c>
       <c r="F33" s="5">
-        <v>58</v>
+        <v>122</v>
       </c>
       <c r="G33" s="5">
-        <v>60</v>
+        <v>132</v>
       </c>
       <c r="H33" s="5">
-        <v>62</v>
+        <v>142</v>
       </c>
       <c r="I33" s="5">
-        <v>63</v>
+        <v>151</v>
       </c>
     </row>
     <row r="34" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C34" s="5">
-        <v>57</v>
+        <v>105</v>
       </c>
       <c r="D34" s="5">
-        <v>61</v>
+        <v>117</v>
       </c>
       <c r="E34" s="5">
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="F34" s="5">
-        <v>68</v>
+        <v>140</v>
       </c>
       <c r="G34" s="5">
-        <v>70</v>
+        <v>150</v>
       </c>
       <c r="H34" s="5">
-        <v>72</v>
+        <v>160</v>
       </c>
       <c r="I34" s="5">
-        <v>74</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>